<commit_message>
PID and variation 1
improved variation 1 but not good
started implementing PID
added if for decision variation 1 or PID
</commit_message>
<xml_diff>
--- a/Perception/Lichtsensor.xlsx
+++ b/Perception/Lichtsensor.xlsx
@@ -1,17 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Christoph/Documents/workspace/HSAMR/Perception/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -96,7 +107,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -169,25 +180,25 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -196,33 +207,33 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -230,66 +241,66 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
@@ -301,16 +312,16 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -318,23 +329,23 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -370,34 +381,34 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -405,7 +416,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -719,19 +730,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="14" max="14" width="24.75" customWidth="1"/>
+    <col min="14" max="14" width="24.6640625" customWidth="1"/>
     <col min="15" max="15" width="23" customWidth="1"/>
-    <col min="16" max="16" width="11.875" customWidth="1"/>
+    <col min="16" max="16" width="11.83203125" customWidth="1"/>
     <col min="17" max="17" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="3"/>
       <c r="C1" s="21" t="s">
         <v>6</v>
@@ -745,12 +756,12 @@
       <c r="K1" s="21"/>
       <c r="L1" s="21"/>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -760,10 +771,10 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="19" t="s">
         <v>4</v>
       </c>
       <c r="L2" s="6" t="s">
@@ -773,7 +784,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="10"/>
       <c r="B3" s="5" t="s">
         <v>0</v>
@@ -803,7 +814,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="5"/>
       <c r="C4" s="7">
@@ -829,7 +840,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
       <c r="B5" s="5"/>
       <c r="C5" s="7">
@@ -855,7 +866,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
       <c r="B6" s="5"/>
       <c r="C6" s="7">
@@ -881,7 +892,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="6"/>
       <c r="C7" s="8">
@@ -906,14 +917,14 @@
       <c r="L7" s="6">
         <v>33</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="N7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-    </row>
-    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+    </row>
+    <row r="8" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="5"/>
       <c r="C8" s="7"/>
@@ -927,18 +938,18 @@
       <c r="K8" s="7"/>
       <c r="L8" s="5"/>
       <c r="M8" s="10"/>
-      <c r="N8" s="17" t="s">
+      <c r="N8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="O8" s="18"/>
-      <c r="P8" s="19" t="s">
+      <c r="O8" s="17"/>
+      <c r="P8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="Q8" s="20" t="s">
+      <c r="Q8" s="19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
       <c r="B9" s="5" t="s">
         <v>1</v>
@@ -981,7 +992,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="5"/>
       <c r="C10" s="7">
@@ -1007,18 +1018,18 @@
         <v>33</v>
       </c>
       <c r="M10" s="4"/>
-      <c r="N10" s="16" t="s">
+      <c r="N10" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16">
+      <c r="O10" s="15"/>
+      <c r="P10" s="15">
         <v>41</v>
       </c>
       <c r="Q10" s="2">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
       <c r="B11" s="5"/>
       <c r="C11" s="7">
@@ -1053,11 +1064,11 @@
       <c r="P11" s="9">
         <v>29</v>
       </c>
-      <c r="Q11" s="13">
+      <c r="Q11" s="12">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="5"/>
       <c r="C12" s="7">
@@ -1083,18 +1094,18 @@
         <v>34</v>
       </c>
       <c r="M12" s="4"/>
-      <c r="N12" s="16" t="s">
+      <c r="N12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14">
+      <c r="O12" s="13"/>
+      <c r="P12" s="13">
         <v>29</v>
       </c>
       <c r="Q12" s="1">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8">
@@ -1123,15 +1134,15 @@
       <c r="N13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16">
+      <c r="O13" s="15"/>
+      <c r="P13" s="15">
         <v>59</v>
       </c>
       <c r="Q13" s="2">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="5"/>
       <c r="C14" s="7"/>
@@ -1151,14 +1162,14 @@
       <c r="O14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="P14" s="13">
+      <c r="P14" s="12">
         <v>54</v>
       </c>
       <c r="Q14" s="9">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="5" t="s">
         <v>2</v>
@@ -1199,7 +1210,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
       <c r="B16" s="5"/>
       <c r="C16" s="7">
@@ -1225,20 +1236,20 @@
         <v>33</v>
       </c>
       <c r="M16" s="10"/>
-      <c r="N16" s="12" t="s">
+      <c r="N16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="O16" s="15" t="s">
+      <c r="O16" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="P16" s="15">
+      <c r="P16" s="14">
         <v>54</v>
       </c>
-      <c r="Q16" s="15" t="s">
+      <c r="Q16" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
       <c r="B17" s="5"/>
       <c r="C17" s="7">
@@ -1275,7 +1286,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
       <c r="B18" s="5"/>
       <c r="C18" s="7">
@@ -1301,7 +1312,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8">
@@ -1327,7 +1338,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>23</v>
       </c>

</xml_diff>